<commit_message>
Done 1-2 in nervous
</commit_message>
<xml_diff>
--- a/Report/Result.xlsx
+++ b/Report/Result.xlsx
@@ -1,40 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenbaolong/Desktop/Không phải nháp/DataMining-Lab3/Report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\HCMUS\Handout\2020-2021\HK1\Data Mining\DataMining-Lab3\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{301B18B3-99B8-044F-9A91-275E4CF989E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB580CE-D3D6-47C6-9858-7287C8614246}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14620" xr2:uid="{A766BBC3-788F-6542-BEF6-FAF04BEACC0C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A766BBC3-788F-6542-BEF6-FAF04BEACC0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="27">
   <si>
     <t>Loại thực nghiệm</t>
   </si>
@@ -110,6 +101,12 @@
   </si>
   <si>
     <t>Giải thích về file afterPreProcess.csv: File .csv này là kết quả của quá trình tiển xử lý file hawks.csv</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Cross-Validation với 10 folds</t>
   </si>
 </sst>
 </file>
@@ -171,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -194,56 +191,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -251,9 +206,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -266,11 +218,18 @@
     <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -278,19 +237,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Accent5" xfId="2" builtinId="48"/>
@@ -607,619 +562,659 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC24104B-79AB-AC40-BB99-DDA6BA15E5DF}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.796875" customWidth="1"/>
+    <col min="4" max="4" width="23.19921875" customWidth="1"/>
+    <col min="5" max="5" width="24.796875" customWidth="1"/>
+    <col min="6" max="6" width="26" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+    <row r="4" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>0.982379</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+    <row r="5" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>0.98017600000000005</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+    <row r="6" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>0.97734600000000005</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+    <row r="7" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+    <row r="8" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="I8" s="18" t="s">
+      <c r="F8" s="14"/>
+      <c r="I8" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+    <row r="9" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="H9" s="18" t="s">
+      <c r="F9" s="14"/>
+      <c r="H9" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>7</v>
-      </c>
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="7">
         <v>0.99449299999999996</v>
       </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>0.982379</v>
       </c>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>0.97411000000000003</v>
       </c>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="8">
         <v>0.98788500000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="8">
         <v>0.98788500000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>12</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="8">
         <v>0.98705500000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <v>14</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="8">
         <v>0.62995599999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="C18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="8">
         <v>0.48220099999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="C19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="8">
         <v>0.982379</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="8">
         <v>0.97577100000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="8">
         <v>0.96440099999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
         <v>19</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="5">
         <v>0.97356799999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>20</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="5">
         <v>0.96806199999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>21</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="5">
         <v>0.96116500000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
         <v>22</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
         <v>23</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="5">
         <v>0.65198199999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>24</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="5">
         <v>0.57281599999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>25</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="5">
         <v>0.982379</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
         <v>26</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="C29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="5">
         <v>0.969163</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
         <v>27</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="5">
         <v>0.967638</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="15">
+        <v>28</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="16">
+        <v>0.90749999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="15">
+        <v>29</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="17">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>